<commit_message>
up css monitoring log sheet
</commit_message>
<xml_diff>
--- a/library/cssPMLReport.xlsx
+++ b/library/cssPMLReport.xlsx
@@ -307,6 +307,10 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -314,7 +318,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -323,9 +326,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -794,7 +794,7 @@
   <dimension ref="A1:Y979"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageLayout" zoomScaleNormal="80" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="J21" sqref="J21"/>
+      <selection activeCell="M17" sqref="M17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -876,28 +876,28 @@
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
-      <c r="D3" s="14"/>
-      <c r="E3" s="15"/>
-      <c r="F3" s="15"/>
-      <c r="G3" s="15"/>
-      <c r="H3" s="15"/>
-      <c r="I3" s="15"/>
-      <c r="J3" s="15"/>
-      <c r="K3" s="15"/>
-      <c r="L3" s="15"/>
-      <c r="M3" s="15"/>
-      <c r="N3" s="15"/>
-      <c r="O3" s="15"/>
-      <c r="P3" s="15"/>
-      <c r="Q3" s="15"/>
-      <c r="R3" s="15"/>
-      <c r="S3" s="15"/>
-      <c r="T3" s="15"/>
-      <c r="U3" s="15"/>
-      <c r="V3" s="15"/>
-      <c r="W3" s="15"/>
-      <c r="X3" s="15"/>
-      <c r="Y3" s="15"/>
+      <c r="D3" s="16"/>
+      <c r="E3" s="17"/>
+      <c r="F3" s="17"/>
+      <c r="G3" s="17"/>
+      <c r="H3" s="17"/>
+      <c r="I3" s="17"/>
+      <c r="J3" s="17"/>
+      <c r="K3" s="17"/>
+      <c r="L3" s="17"/>
+      <c r="M3" s="17"/>
+      <c r="N3" s="17"/>
+      <c r="O3" s="17"/>
+      <c r="P3" s="17"/>
+      <c r="Q3" s="17"/>
+      <c r="R3" s="17"/>
+      <c r="S3" s="17"/>
+      <c r="T3" s="17"/>
+      <c r="U3" s="17"/>
+      <c r="V3" s="17"/>
+      <c r="W3" s="17"/>
+      <c r="X3" s="17"/>
+      <c r="Y3" s="17"/>
     </row>
     <row r="4" spans="1:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1"/>
@@ -954,24 +954,24 @@
       <c r="Y5" s="1"/>
     </row>
     <row r="6" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="19" t="s">
+      <c r="A6" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="B6" s="15"/>
-      <c r="C6" s="15"/>
-      <c r="D6" s="15"/>
-      <c r="E6" s="15"/>
-      <c r="F6" s="15"/>
-      <c r="G6" s="15"/>
-      <c r="H6" s="15"/>
-      <c r="I6" s="15"/>
-      <c r="J6" s="15"/>
-      <c r="K6" s="15"/>
-      <c r="L6" s="15"/>
-      <c r="M6" s="15"/>
-      <c r="N6" s="15"/>
-      <c r="O6" s="15"/>
-      <c r="P6" s="15"/>
+      <c r="B6" s="17"/>
+      <c r="C6" s="17"/>
+      <c r="D6" s="17"/>
+      <c r="E6" s="17"/>
+      <c r="F6" s="17"/>
+      <c r="G6" s="17"/>
+      <c r="H6" s="17"/>
+      <c r="I6" s="17"/>
+      <c r="J6" s="17"/>
+      <c r="K6" s="17"/>
+      <c r="L6" s="17"/>
+      <c r="M6" s="17"/>
+      <c r="N6" s="17"/>
+      <c r="O6" s="17"/>
+      <c r="P6" s="17"/>
       <c r="Q6" s="1"/>
       <c r="R6" s="1"/>
       <c r="S6" s="1"/>
@@ -983,24 +983,24 @@
       <c r="Y6" s="1"/>
     </row>
     <row r="7" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="19" t="s">
+      <c r="A7" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="B7" s="15"/>
-      <c r="C7" s="15"/>
-      <c r="D7" s="15"/>
-      <c r="E7" s="15"/>
-      <c r="F7" s="15"/>
-      <c r="G7" s="15"/>
-      <c r="H7" s="15"/>
-      <c r="I7" s="15"/>
-      <c r="J7" s="15"/>
-      <c r="K7" s="15"/>
-      <c r="L7" s="15"/>
-      <c r="M7" s="15"/>
-      <c r="N7" s="15"/>
-      <c r="O7" s="15"/>
-      <c r="P7" s="15"/>
+      <c r="B7" s="17"/>
+      <c r="C7" s="17"/>
+      <c r="D7" s="17"/>
+      <c r="E7" s="17"/>
+      <c r="F7" s="17"/>
+      <c r="G7" s="17"/>
+      <c r="H7" s="17"/>
+      <c r="I7" s="17"/>
+      <c r="J7" s="17"/>
+      <c r="K7" s="17"/>
+      <c r="L7" s="17"/>
+      <c r="M7" s="17"/>
+      <c r="N7" s="17"/>
+      <c r="O7" s="17"/>
+      <c r="P7" s="17"/>
       <c r="Q7" s="1"/>
       <c r="R7" s="1"/>
       <c r="S7" s="1"/>
@@ -1012,24 +1012,24 @@
       <c r="Y7" s="1"/>
     </row>
     <row r="8" spans="1:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="20" t="s">
+      <c r="A8" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="B8" s="15"/>
-      <c r="C8" s="15"/>
-      <c r="D8" s="15"/>
-      <c r="E8" s="15"/>
-      <c r="F8" s="15"/>
-      <c r="G8" s="15"/>
-      <c r="H8" s="15"/>
-      <c r="I8" s="15"/>
-      <c r="J8" s="15"/>
-      <c r="K8" s="15"/>
-      <c r="L8" s="15"/>
-      <c r="M8" s="15"/>
-      <c r="N8" s="15"/>
-      <c r="O8" s="15"/>
-      <c r="P8" s="15"/>
+      <c r="B8" s="17"/>
+      <c r="C8" s="17"/>
+      <c r="D8" s="17"/>
+      <c r="E8" s="17"/>
+      <c r="F8" s="17"/>
+      <c r="G8" s="17"/>
+      <c r="H8" s="17"/>
+      <c r="I8" s="17"/>
+      <c r="J8" s="17"/>
+      <c r="K8" s="17"/>
+      <c r="L8" s="17"/>
+      <c r="M8" s="17"/>
+      <c r="N8" s="17"/>
+      <c r="O8" s="17"/>
+      <c r="P8" s="17"/>
       <c r="Q8" s="1"/>
       <c r="R8" s="1"/>
       <c r="S8" s="1"/>
@@ -1068,13 +1068,13 @@
       <c r="Y9" s="1"/>
     </row>
     <row r="10" spans="1:25" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="16" t="s">
+      <c r="A10" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B10" s="18" t="s">
+      <c r="B10" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="C10" s="18" t="s">
+      <c r="C10" s="19" t="s">
         <v>2</v>
       </c>
       <c r="D10" s="25" t="s">
@@ -1093,7 +1093,7 @@
       </c>
       <c r="N10" s="23"/>
       <c r="O10" s="24"/>
-      <c r="P10" s="18" t="s">
+      <c r="P10" s="19" t="s">
         <v>5</v>
       </c>
       <c r="Q10" s="2"/>
@@ -1107,46 +1107,46 @@
       <c r="Y10" s="2"/>
     </row>
     <row r="11" spans="1:25" ht="76.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="17"/>
-      <c r="B11" s="17"/>
-      <c r="C11" s="17"/>
-      <c r="D11" s="21" t="s">
+      <c r="A11" s="15"/>
+      <c r="B11" s="15"/>
+      <c r="C11" s="15"/>
+      <c r="D11" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="E11" s="21" t="s">
+      <c r="E11" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="F11" s="21" t="s">
+      <c r="F11" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="G11" s="21" t="s">
+      <c r="G11" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="H11" s="21" t="s">
+      <c r="H11" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="I11" s="21" t="s">
+      <c r="I11" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="J11" s="21" t="s">
+      <c r="J11" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="K11" s="21" t="s">
+      <c r="K11" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="L11" s="21" t="s">
+      <c r="L11" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="M11" s="18" t="s">
+      <c r="M11" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="N11" s="18" t="s">
+      <c r="N11" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="O11" s="18" t="s">
+      <c r="O11" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="P11" s="17"/>
+      <c r="P11" s="15"/>
       <c r="Q11" s="2"/>
       <c r="R11" s="2"/>
       <c r="S11" s="2"/>
@@ -1158,22 +1158,22 @@
       <c r="Y11" s="2"/>
     </row>
     <row r="12" spans="1:25" ht="33.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="17"/>
-      <c r="B12" s="17"/>
-      <c r="C12" s="17"/>
-      <c r="D12" s="17"/>
-      <c r="E12" s="17"/>
-      <c r="F12" s="17"/>
-      <c r="G12" s="17"/>
-      <c r="H12" s="17"/>
-      <c r="I12" s="17"/>
-      <c r="J12" s="17"/>
-      <c r="K12" s="17"/>
-      <c r="L12" s="17"/>
-      <c r="M12" s="17"/>
-      <c r="N12" s="17"/>
-      <c r="O12" s="17"/>
-      <c r="P12" s="17"/>
+      <c r="A12" s="15"/>
+      <c r="B12" s="15"/>
+      <c r="C12" s="15"/>
+      <c r="D12" s="15"/>
+      <c r="E12" s="15"/>
+      <c r="F12" s="15"/>
+      <c r="G12" s="15"/>
+      <c r="H12" s="15"/>
+      <c r="I12" s="15"/>
+      <c r="J12" s="15"/>
+      <c r="K12" s="15"/>
+      <c r="L12" s="15"/>
+      <c r="M12" s="15"/>
+      <c r="N12" s="15"/>
+      <c r="O12" s="15"/>
+      <c r="P12" s="15"/>
       <c r="Q12" s="3"/>
       <c r="R12" s="3"/>
       <c r="S12" s="3"/>
@@ -1222,9 +1222,7 @@
         <f>AVERAGE(D13:K13)</f>
         <v>5</v>
       </c>
-      <c r="M13" s="8">
-        <v>1</v>
-      </c>
+      <c r="M13" s="8"/>
       <c r="N13" s="9"/>
       <c r="O13" s="9"/>
       <c r="P13" s="9"/>
@@ -27322,13 +27320,6 @@
     </row>
   </sheetData>
   <mergeCells count="22">
-    <mergeCell ref="K11:K12"/>
-    <mergeCell ref="L11:L12"/>
-    <mergeCell ref="D11:D12"/>
-    <mergeCell ref="E11:E12"/>
-    <mergeCell ref="F11:F12"/>
-    <mergeCell ref="G11:G12"/>
-    <mergeCell ref="H11:H12"/>
     <mergeCell ref="D3:Y3"/>
     <mergeCell ref="A10:A12"/>
     <mergeCell ref="B10:B12"/>
@@ -27344,6 +27335,13 @@
     <mergeCell ref="O11:O12"/>
     <mergeCell ref="C10:C12"/>
     <mergeCell ref="D10:L10"/>
+    <mergeCell ref="K11:K12"/>
+    <mergeCell ref="L11:L12"/>
+    <mergeCell ref="D11:D12"/>
+    <mergeCell ref="E11:E12"/>
+    <mergeCell ref="F11:F12"/>
+    <mergeCell ref="G11:G12"/>
+    <mergeCell ref="H11:H12"/>
   </mergeCells>
   <phoneticPr fontId="9" type="noConversion"/>
   <pageMargins left="0.59055118110236227" right="0.31496062992125984" top="0.70866141732283472" bottom="0.51181102362204722" header="0" footer="0"/>

</xml_diff>